<commit_message>
create buttons to add item to favourite or shopping items
</commit_message>
<xml_diff>
--- a/src/main/resources/database/favourite_items.xlsx
+++ b/src/main/resources/database/favourite_items.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositories\clothing-store\src\main\resources\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C05149A5-9153-4463-8D86-5816DC6856E2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E7C0E97-8D8E-4929-875C-AC3C8EE85C89}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4500" yWindow="3396" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,15 +17,20 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="0" uniqueCount="0"/>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -337,10 +342,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -361,6 +366,9 @@
       <c r="E1">
         <v>9</v>
       </c>
+      <c r="F1" t="n">
+        <v>58.0</v>
+      </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">

</xml_diff>

<commit_message>
add shop_page to go to shop of item
</commit_message>
<xml_diff>
--- a/src/main/resources/database/favourite_items.xlsx
+++ b/src/main/resources/database/favourite_items.xlsx
@@ -342,7 +342,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G1" sqref="G1"/>
@@ -369,6 +369,9 @@
       <c r="F1" t="n">
         <v>58.0</v>
       </c>
+      <c r="G1" t="n">
+        <v>67.0</v>
+      </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">

</xml_diff>

<commit_message>
add payment in CustomerPage.java for shoppingItems
</commit_message>
<xml_diff>
--- a/src/main/resources/database/favourite_items.xlsx
+++ b/src/main/resources/database/favourite_items.xlsx
@@ -342,7 +342,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G1" sqref="G1"/>
@@ -372,6 +372,12 @@
       <c r="G1" t="n">
         <v>67.0</v>
       </c>
+      <c r="H1" t="n">
+        <v>15.0</v>
+      </c>
+      <c r="I1" t="n">
+        <v>32.0</v>
+      </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">

</xml_diff>

<commit_message>
review all scripts + add interaction with orders as customer
</commit_message>
<xml_diff>
--- a/src/main/resources/database/favourite_items.xlsx
+++ b/src/main/resources/database/favourite_items.xlsx
@@ -342,7 +342,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G1" sqref="G1"/>
@@ -381,6 +381,12 @@
       <c r="J1" t="n">
         <v>96.0</v>
       </c>
+      <c r="K1" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="L1" t="n">
+        <v>90.0</v>
+      </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">

</xml_diff>

<commit_message>
correct some ui things
</commit_message>
<xml_diff>
--- a/src/main/resources/database/favourite_items.xlsx
+++ b/src/main/resources/database/favourite_items.xlsx
@@ -342,7 +342,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G1" sqref="G1"/>
@@ -387,6 +387,9 @@
       <c r="L1" t="n">
         <v>90.0</v>
       </c>
+      <c r="M1" t="n">
+        <v>83.0</v>
+      </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">

</xml_diff>

<commit_message>
add opportunity to delete items as customer
</commit_message>
<xml_diff>
--- a/src/main/resources/database/favourite_items.xlsx
+++ b/src/main/resources/database/favourite_items.xlsx
@@ -342,7 +342,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M3"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G1" sqref="G1"/>
@@ -352,43 +352,40 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B1">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C1">
-        <v>6</v>
-      </c>
-      <c r="D1">
-        <v>8</v>
-      </c>
-      <c r="E1">
         <v>9</v>
       </c>
+      <c r="D1" t="n">
+        <v>58.0</v>
+      </c>
+      <c r="E1" t="n">
+        <v>67.0</v>
+      </c>
       <c r="F1" t="n">
-        <v>58.0</v>
+        <v>15.0</v>
       </c>
       <c r="G1" t="n">
-        <v>67.0</v>
+        <v>4.0</v>
       </c>
       <c r="H1" t="n">
-        <v>15.0</v>
+        <v>83.0</v>
       </c>
       <c r="I1" t="n">
-        <v>32.0</v>
+        <v>34.0</v>
       </c>
       <c r="J1" t="n">
-        <v>96.0</v>
+        <v>106.0</v>
       </c>
       <c r="K1" t="n">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
       <c r="L1" t="n">
-        <v>90.0</v>
-      </c>
-      <c r="M1" t="n">
-        <v>83.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -402,6 +399,11 @@
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>78</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>124.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add settings to account page
</commit_message>
<xml_diff>
--- a/src/main/resources/database/favourite_items.xlsx
+++ b/src/main/resources/database/favourite_items.xlsx
@@ -342,7 +342,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G1" sqref="G1"/>
@@ -370,21 +370,15 @@
         <v>15.0</v>
       </c>
       <c r="G1" t="n">
-        <v>4.0</v>
+        <v>83.0</v>
       </c>
       <c r="H1" t="n">
-        <v>83.0</v>
+        <v>34.0</v>
       </c>
       <c r="I1" t="n">
-        <v>34.0</v>
+        <v>3.0</v>
       </c>
       <c r="J1" t="n">
-        <v>106.0</v>
-      </c>
-      <c r="K1" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="L1" t="n">
         <v>1.0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
implementation of pattern Observer
</commit_message>
<xml_diff>
--- a/src/main/resources/database/favourite_items.xlsx
+++ b/src/main/resources/database/favourite_items.xlsx
@@ -342,7 +342,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G1" sqref="G1"/>
@@ -367,19 +367,13 @@
         <v>67.0</v>
       </c>
       <c r="F1" t="n">
-        <v>15.0</v>
+        <v>3.0</v>
       </c>
       <c r="G1" t="n">
-        <v>83.0</v>
+        <v>1.0</v>
       </c>
       <c r="H1" t="n">
-        <v>34.0</v>
-      </c>
-      <c r="I1" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="J1" t="n">
-        <v>1.0</v>
+        <v>73.0</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -398,6 +392,9 @@
     <row r="7">
       <c r="A7" t="n">
         <v>124.0</v>
+      </c>
+      <c r="B7" t="n">
+        <v>22.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add orderItems + simplify some things
</commit_message>
<xml_diff>
--- a/src/main/resources/database/favourite_items.xlsx
+++ b/src/main/resources/database/favourite_items.xlsx
@@ -342,7 +342,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:Q7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G1" sqref="G1"/>
@@ -350,24 +350,57 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1">
-        <v>6</v>
+    <row r="1">
+      <c r="A1" t="n">
+        <v>11.0</v>
       </c>
       <c r="B1" t="n">
-        <v>58.0</v>
+        <v>16.0</v>
       </c>
       <c r="C1" t="n">
-        <v>67.0</v>
+        <v>31.0</v>
       </c>
       <c r="D1" t="n">
-        <v>3.0</v>
+        <v>32.0</v>
       </c>
       <c r="E1" t="n">
-        <v>1.0</v>
+        <v>28.0</v>
       </c>
       <c r="F1" t="n">
+        <v>33.0</v>
+      </c>
+      <c r="G1" t="n">
+        <v>34.0</v>
+      </c>
+      <c r="H1" t="n">
+        <v>39.0</v>
+      </c>
+      <c r="I1" t="n">
+        <v>40.0</v>
+      </c>
+      <c r="J1" t="n">
+        <v>41.0</v>
+      </c>
+      <c r="K1" t="n">
+        <v>45.0</v>
+      </c>
+      <c r="L1" t="n">
+        <v>46.0</v>
+      </c>
+      <c r="M1" t="n">
+        <v>70.0</v>
+      </c>
+      <c r="N1" t="n">
         <v>73.0</v>
+      </c>
+      <c r="O1" t="n">
+        <v>79.0</v>
+      </c>
+      <c r="P1" t="n">
+        <v>82.0</v>
+      </c>
+      <c r="Q1" t="n">
+        <v>104.0</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>